<commit_message>
Update Data Scientists Salary - By Industry.xlsx
</commit_message>
<xml_diff>
--- a/Project1 - Visualizing Data Scientists Salaries(USA)/Input/Data Scientists Salary - By Industry.xlsx
+++ b/Project1 - Visualizing Data Scientists Salaries(USA)/Input/Data Scientists Salary - By Industry.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10908"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gagandeepsingh/Desktop/Gagan/Data Science - Projects/Archive APIs &amp; Notes/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gagandeepsingh/Desktop/Gagan/Data Science - Projects/Github/Data-Visualization-Projects-Tableau/Project1 - Visualizing Data Scientists Salaries(USA)/Input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DCB8E2E-DE6C-3241-B6F8-FDB0B14A9D63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BB089AE-1AE0-5F43-9C68-500C13D394B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="29400" windowHeight="17340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -986,7 +986,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -998,36 +998,14 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="1">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -14783,49 +14761,49 @@
       <c r="A269" s="4" t="s">
         <v>274</v>
       </c>
-      <c r="B269" s="6">
+      <c r="B269" s="4">
         <v>70</v>
       </c>
-      <c r="C269" s="6">
+      <c r="C269" s="4">
         <v>26.4</v>
       </c>
-      <c r="D269" s="6">
+      <c r="D269" s="4">
         <v>56.31</v>
       </c>
-      <c r="E269" s="6">
+      <c r="E269" s="4">
         <v>117120</v>
       </c>
-      <c r="F269" s="6">
+      <c r="F269" s="4">
         <v>9.6</v>
       </c>
-      <c r="G269" s="6">
+      <c r="G269" s="4">
         <v>37.5</v>
       </c>
-      <c r="H269" s="6">
+      <c r="H269" s="4">
         <v>42.29</v>
       </c>
-      <c r="I269" s="6">
+      <c r="I269" s="4">
         <v>47.96</v>
       </c>
-      <c r="J269" s="6">
+      <c r="J269" s="4">
         <v>52.6</v>
       </c>
-      <c r="K269" s="6">
+      <c r="K269" s="4">
         <v>105.04</v>
       </c>
-      <c r="L269" s="6">
+      <c r="L269" s="4">
         <v>78000</v>
       </c>
-      <c r="M269" s="6">
+      <c r="M269" s="4">
         <v>87960</v>
       </c>
-      <c r="N269" s="6">
+      <c r="N269" s="4">
         <v>99750</v>
       </c>
-      <c r="O269" s="6">
+      <c r="O269" s="4">
         <v>109400</v>
       </c>
-      <c r="P269" s="6">
+      <c r="P269" s="4">
         <v>218470</v>
       </c>
     </row>
@@ -14833,49 +14811,49 @@
       <c r="A270" t="s">
         <v>275</v>
       </c>
-      <c r="B270" s="7">
+      <c r="B270">
         <v>2130</v>
       </c>
-      <c r="C270" s="7">
+      <c r="C270">
         <v>6.8</v>
       </c>
-      <c r="D270" s="7">
+      <c r="D270">
         <v>44.91</v>
       </c>
-      <c r="E270" s="7">
+      <c r="E270">
         <v>93400</v>
       </c>
-      <c r="F270" s="7">
+      <c r="F270">
         <v>5</v>
       </c>
-      <c r="G270" s="7">
+      <c r="G270">
         <v>23.93</v>
       </c>
-      <c r="H270" s="7">
+      <c r="H270">
         <v>30.67</v>
       </c>
-      <c r="I270" s="7">
+      <c r="I270">
         <v>40.090000000000003</v>
       </c>
-      <c r="J270" s="7">
+      <c r="J270">
         <v>53.08</v>
       </c>
-      <c r="K270" s="7">
+      <c r="K270">
         <v>72.12</v>
       </c>
-      <c r="L270" s="7">
+      <c r="L270">
         <v>49780</v>
       </c>
-      <c r="M270" s="7">
+      <c r="M270">
         <v>63790</v>
       </c>
-      <c r="N270" s="7">
+      <c r="N270">
         <v>83390</v>
       </c>
-      <c r="O270" s="7">
+      <c r="O270">
         <v>110410</v>
       </c>
-      <c r="P270" s="7">
+      <c r="P270">
         <v>150000</v>
       </c>
     </row>
@@ -14883,49 +14861,49 @@
       <c r="A271" t="s">
         <v>276</v>
       </c>
-      <c r="B271" s="7">
+      <c r="B271">
         <v>50</v>
       </c>
-      <c r="C271" s="7">
+      <c r="C271">
         <v>22.2</v>
       </c>
-      <c r="D271" s="7">
+      <c r="D271">
         <v>37.659999999999997</v>
       </c>
-      <c r="E271" s="7">
+      <c r="E271">
         <v>78320</v>
       </c>
-      <c r="F271" s="7">
+      <c r="F271">
         <v>4</v>
       </c>
-      <c r="G271" s="7">
+      <c r="G271">
         <v>26.88</v>
       </c>
-      <c r="H271" s="7">
+      <c r="H271">
         <v>28.07</v>
       </c>
-      <c r="I271" s="7">
+      <c r="I271">
         <v>37.520000000000003</v>
       </c>
-      <c r="J271" s="7">
+      <c r="J271">
         <v>46.11</v>
       </c>
-      <c r="K271" s="7">
+      <c r="K271">
         <v>47.84</v>
       </c>
-      <c r="L271" s="7">
+      <c r="L271">
         <v>55920</v>
       </c>
-      <c r="M271" s="7">
+      <c r="M271">
         <v>58380</v>
       </c>
-      <c r="N271" s="7">
+      <c r="N271">
         <v>78050</v>
       </c>
-      <c r="O271" s="7">
+      <c r="O271">
         <v>95920</v>
       </c>
-      <c r="P271" s="7">
+      <c r="P271">
         <v>99510</v>
       </c>
     </row>
@@ -14933,49 +14911,49 @@
       <c r="A272" t="s">
         <v>277</v>
       </c>
-      <c r="B272" s="7">
+      <c r="B272">
         <v>450</v>
       </c>
-      <c r="C272" s="7">
+      <c r="C272">
         <v>9.9</v>
       </c>
-      <c r="D272" s="7">
+      <c r="D272">
         <v>44.62</v>
       </c>
-      <c r="E272" s="7">
+      <c r="E272">
         <v>92820</v>
       </c>
-      <c r="F272" s="7">
+      <c r="F272">
         <v>4.5</v>
       </c>
-      <c r="G272" s="7">
+      <c r="G272">
         <v>26.21</v>
       </c>
-      <c r="H272" s="7">
+      <c r="H272">
         <v>31.7</v>
       </c>
-      <c r="I272" s="7">
+      <c r="I272">
         <v>38.89</v>
       </c>
-      <c r="J272" s="7">
+      <c r="J272">
         <v>52.86</v>
       </c>
-      <c r="K272" s="7">
+      <c r="K272">
         <v>72</v>
       </c>
-      <c r="L272" s="7">
+      <c r="L272">
         <v>54520</v>
       </c>
-      <c r="M272" s="7">
+      <c r="M272">
         <v>65940</v>
       </c>
-      <c r="N272" s="7">
+      <c r="N272">
         <v>80890</v>
       </c>
-      <c r="O272" s="7">
+      <c r="O272">
         <v>109950</v>
       </c>
-      <c r="P272" s="7">
+      <c r="P272">
         <v>149760</v>
       </c>
     </row>
@@ -14983,49 +14961,49 @@
       <c r="A273" t="s">
         <v>278</v>
       </c>
-      <c r="B273" s="7">
+      <c r="B273">
         <v>480</v>
       </c>
-      <c r="C273" s="7">
+      <c r="C273">
         <v>14.2</v>
       </c>
-      <c r="D273" s="7">
+      <c r="D273">
         <v>41.59</v>
       </c>
-      <c r="E273" s="7">
+      <c r="E273">
         <v>86510</v>
       </c>
-      <c r="F273" s="7">
+      <c r="F273">
         <v>6</v>
       </c>
-      <c r="G273" s="7">
+      <c r="G273">
         <v>26.75</v>
       </c>
-      <c r="H273" s="7">
+      <c r="H273">
         <v>30.52</v>
       </c>
-      <c r="I273" s="7">
+      <c r="I273">
         <v>37.78</v>
       </c>
-      <c r="J273" s="7">
+      <c r="J273">
         <v>48.7</v>
       </c>
-      <c r="K273" s="7">
+      <c r="K273">
         <v>62.34</v>
       </c>
-      <c r="L273" s="7">
+      <c r="L273">
         <v>55640</v>
       </c>
-      <c r="M273" s="7">
+      <c r="M273">
         <v>63490</v>
       </c>
-      <c r="N273" s="7">
+      <c r="N273">
         <v>78580</v>
       </c>
-      <c r="O273" s="7">
+      <c r="O273">
         <v>101300</v>
       </c>
-      <c r="P273" s="7">
+      <c r="P273">
         <v>129670</v>
       </c>
     </row>
@@ -15033,49 +15011,49 @@
       <c r="A274" t="s">
         <v>279</v>
       </c>
-      <c r="B274" s="7">
+      <c r="B274">
         <v>150</v>
       </c>
-      <c r="C274" s="7">
+      <c r="C274">
         <v>24.2</v>
       </c>
-      <c r="D274" s="7">
+      <c r="D274">
         <v>34.799999999999997</v>
       </c>
-      <c r="E274" s="7">
+      <c r="E274">
         <v>72380</v>
       </c>
-      <c r="F274" s="7">
+      <c r="F274">
         <v>6.2</v>
       </c>
-      <c r="G274" s="7">
+      <c r="G274">
         <v>24.32</v>
       </c>
-      <c r="H274" s="7">
+      <c r="H274">
         <v>29.56</v>
       </c>
-      <c r="I274" s="7">
+      <c r="I274">
         <v>31.17</v>
       </c>
-      <c r="J274" s="7">
+      <c r="J274">
         <v>41.33</v>
       </c>
-      <c r="K274" s="7">
+      <c r="K274">
         <v>47.22</v>
       </c>
-      <c r="L274" s="7">
+      <c r="L274">
         <v>50590</v>
       </c>
-      <c r="M274" s="7">
+      <c r="M274">
         <v>61470</v>
       </c>
-      <c r="N274" s="7">
+      <c r="N274">
         <v>64830</v>
       </c>
-      <c r="O274" s="7">
+      <c r="O274">
         <v>85960</v>
       </c>
-      <c r="P274" s="7">
+      <c r="P274">
         <v>98210</v>
       </c>
     </row>
@@ -15083,49 +15061,49 @@
       <c r="A275" t="s">
         <v>280</v>
       </c>
-      <c r="B275" s="7">
+      <c r="B275">
         <v>990</v>
       </c>
-      <c r="C275" s="7">
+      <c r="C275">
         <v>12.3</v>
       </c>
-      <c r="D275" s="7">
+      <c r="D275">
         <v>48.51</v>
       </c>
-      <c r="E275" s="7">
+      <c r="E275">
         <v>100900</v>
       </c>
-      <c r="F275" s="7">
+      <c r="F275">
         <v>5.9</v>
       </c>
-      <c r="G275" s="7">
+      <c r="G275">
         <v>20.36</v>
       </c>
-      <c r="H275" s="7">
+      <c r="H275">
         <v>34.26</v>
       </c>
-      <c r="I275" s="7">
+      <c r="I275">
         <v>44.93</v>
       </c>
-      <c r="J275" s="7">
+      <c r="J275">
         <v>59.79</v>
       </c>
-      <c r="K275" s="7">
+      <c r="K275">
         <v>84.91</v>
       </c>
-      <c r="L275" s="7">
+      <c r="L275">
         <v>42350</v>
       </c>
-      <c r="M275" s="7">
+      <c r="M275">
         <v>71250</v>
       </c>
-      <c r="N275" s="7">
+      <c r="N275">
         <v>93460</v>
       </c>
-      <c r="O275" s="7">
+      <c r="O275">
         <v>124370</v>
       </c>
-      <c r="P275" s="7">
+      <c r="P275">
         <v>176610</v>
       </c>
     </row>
@@ -15133,49 +15111,49 @@
       <c r="A276" t="s">
         <v>281</v>
       </c>
-      <c r="B276" s="7">
+      <c r="B276">
         <v>70</v>
       </c>
-      <c r="C276" s="7">
+      <c r="C276">
         <v>40.200000000000003</v>
       </c>
-      <c r="D276" s="7">
+      <c r="D276">
         <v>46.32</v>
       </c>
-      <c r="E276" s="7">
+      <c r="E276">
         <v>96350</v>
       </c>
-      <c r="F276" s="7">
+      <c r="F276">
         <v>3.5</v>
       </c>
-      <c r="G276" s="7">
+      <c r="G276">
         <v>33.25</v>
       </c>
-      <c r="H276" s="7">
+      <c r="H276">
         <v>37.92</v>
       </c>
-      <c r="I276" s="7">
+      <c r="I276">
         <v>46.94</v>
       </c>
-      <c r="J276" s="7">
+      <c r="J276">
         <v>51.98</v>
       </c>
-      <c r="K276" s="7">
+      <c r="K276">
         <v>60.49</v>
       </c>
-      <c r="L276" s="7">
+      <c r="L276">
         <v>69170</v>
       </c>
-      <c r="M276" s="7">
+      <c r="M276">
         <v>78880</v>
       </c>
-      <c r="N276" s="7">
+      <c r="N276">
         <v>97630</v>
       </c>
-      <c r="O276" s="7">
+      <c r="O276">
         <v>108120</v>
       </c>
-      <c r="P276" s="7">
+      <c r="P276">
         <v>125830</v>
       </c>
     </row>
@@ -15183,49 +15161,49 @@
       <c r="A277" t="s">
         <v>282</v>
       </c>
-      <c r="B277" s="7">
+      <c r="B277">
         <v>3470</v>
       </c>
-      <c r="C277" s="7">
+      <c r="C277">
         <v>1.3</v>
       </c>
-      <c r="D277" s="7">
+      <c r="D277">
         <v>43.17</v>
       </c>
-      <c r="E277" s="7">
+      <c r="E277">
         <v>89800</v>
       </c>
-      <c r="F277" s="7">
+      <c r="F277">
         <v>0.4</v>
       </c>
-      <c r="G277" s="7">
+      <c r="G277">
         <v>27.8</v>
       </c>
-      <c r="H277" s="7">
+      <c r="H277">
         <v>33.92</v>
       </c>
-      <c r="I277" s="7">
+      <c r="I277">
         <v>41.86</v>
       </c>
-      <c r="J277" s="7">
+      <c r="J277">
         <v>48.14</v>
       </c>
-      <c r="K277" s="7">
+      <c r="K277">
         <v>60.11</v>
       </c>
-      <c r="L277" s="7">
+      <c r="L277">
         <v>57820</v>
       </c>
-      <c r="M277" s="7">
+      <c r="M277">
         <v>70550</v>
       </c>
-      <c r="N277" s="7">
+      <c r="N277">
         <v>87070</v>
       </c>
-      <c r="O277" s="7">
+      <c r="O277">
         <v>100130</v>
       </c>
-      <c r="P277" s="7">
+      <c r="P277">
         <v>125030</v>
       </c>
     </row>
@@ -15233,49 +15211,49 @@
       <c r="A278" t="s">
         <v>283</v>
       </c>
-      <c r="B278" s="7">
+      <c r="B278">
         <v>3470</v>
       </c>
-      <c r="C278" s="7">
+      <c r="C278">
         <v>1.3</v>
       </c>
-      <c r="D278" s="7">
+      <c r="D278">
         <v>43.17</v>
       </c>
-      <c r="E278" s="7">
+      <c r="E278">
         <v>89800</v>
       </c>
-      <c r="F278" s="7">
+      <c r="F278">
         <v>0.4</v>
       </c>
-      <c r="G278" s="7">
+      <c r="G278">
         <v>27.8</v>
       </c>
-      <c r="H278" s="7">
+      <c r="H278">
         <v>33.92</v>
       </c>
-      <c r="I278" s="7">
+      <c r="I278">
         <v>41.86</v>
       </c>
-      <c r="J278" s="7">
+      <c r="J278">
         <v>48.14</v>
       </c>
-      <c r="K278" s="7">
+      <c r="K278">
         <v>60.11</v>
       </c>
-      <c r="L278" s="7">
+      <c r="L278">
         <v>57820</v>
       </c>
-      <c r="M278" s="7">
+      <c r="M278">
         <v>70550</v>
       </c>
-      <c r="N278" s="7">
+      <c r="N278">
         <v>87070</v>
       </c>
-      <c r="O278" s="7">
+      <c r="O278">
         <v>100130</v>
       </c>
-      <c r="P278" s="7">
+      <c r="P278">
         <v>125030</v>
       </c>
     </row>
@@ -15283,49 +15261,49 @@
       <c r="A279" t="s">
         <v>284</v>
       </c>
-      <c r="B279" s="7">
+      <c r="B279">
         <v>7990</v>
       </c>
-      <c r="C279" s="7">
+      <c r="C279">
         <v>1.6</v>
       </c>
-      <c r="D279" s="7">
+      <c r="D279">
         <v>42.6</v>
       </c>
-      <c r="E279" s="7">
+      <c r="E279">
         <v>88600</v>
       </c>
-      <c r="F279" s="7">
+      <c r="F279">
         <v>1.6</v>
       </c>
-      <c r="G279" s="7">
+      <c r="G279">
         <v>25.71</v>
       </c>
-      <c r="H279" s="7">
+      <c r="H279">
         <v>31.76</v>
       </c>
-      <c r="I279" s="7">
+      <c r="I279">
         <v>39.64</v>
       </c>
-      <c r="J279" s="7">
+      <c r="J279">
         <v>49.03</v>
       </c>
-      <c r="K279" s="7">
+      <c r="K279">
         <v>62.59</v>
       </c>
-      <c r="L279" s="7">
+      <c r="L279">
         <v>53480</v>
       </c>
-      <c r="M279" s="7">
+      <c r="M279">
         <v>66060</v>
       </c>
-      <c r="N279" s="7">
+      <c r="N279">
         <v>82460</v>
       </c>
-      <c r="O279" s="7">
+      <c r="O279">
         <v>101980</v>
       </c>
-      <c r="P279" s="7">
+      <c r="P279">
         <v>130180</v>
       </c>
     </row>
@@ -15333,49 +15311,49 @@
       <c r="A280" t="s">
         <v>285</v>
       </c>
-      <c r="B280" s="7">
+      <c r="B280">
         <v>410</v>
       </c>
-      <c r="C280" s="7">
+      <c r="C280">
         <v>0</v>
       </c>
-      <c r="D280" s="7">
+      <c r="D280">
         <v>58.3</v>
       </c>
-      <c r="E280" s="7">
+      <c r="E280">
         <v>121260</v>
       </c>
-      <c r="F280" s="7">
+      <c r="F280">
         <v>0</v>
       </c>
-      <c r="G280" s="7">
+      <c r="G280">
         <v>36.75</v>
       </c>
-      <c r="H280" s="7">
+      <c r="H280">
         <v>45.83</v>
       </c>
-      <c r="I280" s="7">
+      <c r="I280">
         <v>57.82</v>
       </c>
-      <c r="J280" s="7">
+      <c r="J280">
         <v>70</v>
       </c>
-      <c r="K280" s="7">
+      <c r="K280">
         <v>80.58</v>
       </c>
-      <c r="L280" s="7">
+      <c r="L280">
         <v>76440</v>
       </c>
-      <c r="M280" s="7">
+      <c r="M280">
         <v>95330</v>
       </c>
-      <c r="N280" s="7">
+      <c r="N280">
         <v>120270</v>
       </c>
-      <c r="O280" s="7">
+      <c r="O280">
         <v>145600</v>
       </c>
-      <c r="P280" s="7">
+      <c r="P280">
         <v>167610</v>
       </c>
     </row>
@@ -15383,49 +15361,49 @@
       <c r="A281" t="s">
         <v>286</v>
       </c>
-      <c r="B281" s="7">
+      <c r="B281">
         <v>410</v>
       </c>
-      <c r="C281" s="7">
+      <c r="C281">
         <v>0</v>
       </c>
-      <c r="D281" s="7">
+      <c r="D281">
         <v>58.3</v>
       </c>
-      <c r="E281" s="7">
+      <c r="E281">
         <v>121260</v>
       </c>
-      <c r="F281" s="7">
+      <c r="F281">
         <v>0</v>
       </c>
-      <c r="G281" s="7">
+      <c r="G281">
         <v>36.75</v>
       </c>
-      <c r="H281" s="7">
+      <c r="H281">
         <v>45.83</v>
       </c>
-      <c r="I281" s="7">
+      <c r="I281">
         <v>57.82</v>
       </c>
-      <c r="J281" s="7">
+      <c r="J281">
         <v>70</v>
       </c>
-      <c r="K281" s="7">
+      <c r="K281">
         <v>80.58</v>
       </c>
-      <c r="L281" s="7">
+      <c r="L281">
         <v>76440</v>
       </c>
-      <c r="M281" s="7">
+      <c r="M281">
         <v>95330</v>
       </c>
-      <c r="N281" s="7">
+      <c r="N281">
         <v>120270</v>
       </c>
-      <c r="O281" s="7">
+      <c r="O281">
         <v>145600</v>
       </c>
-      <c r="P281" s="7">
+      <c r="P281">
         <v>167610</v>
       </c>
     </row>
@@ -15433,49 +15411,49 @@
       <c r="A282" t="s">
         <v>287</v>
       </c>
-      <c r="B282" s="7">
+      <c r="B282">
         <v>1960</v>
       </c>
-      <c r="C282" s="7">
+      <c r="C282">
         <v>0</v>
       </c>
-      <c r="D282" s="7">
+      <c r="D282">
         <v>41.44</v>
       </c>
-      <c r="E282" s="7">
+      <c r="E282">
         <v>86200</v>
       </c>
-      <c r="F282" s="7">
+      <c r="F282">
         <v>0</v>
       </c>
-      <c r="G282" s="7">
+      <c r="G282">
         <v>30.45</v>
       </c>
-      <c r="H282" s="7">
+      <c r="H282">
         <v>35.090000000000003</v>
       </c>
-      <c r="I282" s="7">
+      <c r="I282">
         <v>41.86</v>
       </c>
-      <c r="J282" s="7">
+      <c r="J282">
         <v>47.03</v>
       </c>
-      <c r="K282" s="7">
+      <c r="K282">
         <v>51.63</v>
       </c>
-      <c r="L282" s="7">
+      <c r="L282">
         <v>63340</v>
       </c>
-      <c r="M282" s="7">
+      <c r="M282">
         <v>72990</v>
       </c>
-      <c r="N282" s="7">
+      <c r="N282">
         <v>87070</v>
       </c>
-      <c r="O282" s="7">
+      <c r="O282">
         <v>97820</v>
       </c>
-      <c r="P282" s="7">
+      <c r="P282">
         <v>107390</v>
       </c>
     </row>
@@ -15483,49 +15461,49 @@
       <c r="A283" t="s">
         <v>288</v>
       </c>
-      <c r="B283" s="7">
+      <c r="B283">
         <v>4900</v>
       </c>
-      <c r="C283" s="7">
+      <c r="C283">
         <v>0.3</v>
       </c>
-      <c r="D283" s="7">
+      <c r="D283">
         <v>41.18</v>
       </c>
-      <c r="E283" s="7">
+      <c r="E283">
         <v>85650</v>
       </c>
-      <c r="F283" s="7">
+      <c r="F283">
         <v>0.3</v>
       </c>
-      <c r="G283" s="7">
+      <c r="G283">
         <v>25.9</v>
       </c>
-      <c r="H283" s="7">
+      <c r="H283">
         <v>32.18</v>
       </c>
-      <c r="I283" s="7">
+      <c r="I283">
         <v>39.64</v>
       </c>
-      <c r="J283" s="7">
+      <c r="J283">
         <v>48.08</v>
       </c>
-      <c r="K283" s="7">
+      <c r="K283">
         <v>57.37</v>
       </c>
-      <c r="L283" s="7">
+      <c r="L283">
         <v>53880</v>
       </c>
-      <c r="M283" s="7">
+      <c r="M283">
         <v>66930</v>
       </c>
-      <c r="N283" s="7">
+      <c r="N283">
         <v>82460</v>
       </c>
-      <c r="O283" s="7">
+      <c r="O283">
         <v>100010</v>
       </c>
-      <c r="P283" s="7">
+      <c r="P283">
         <v>119340</v>
       </c>
     </row>
@@ -15533,49 +15511,49 @@
       <c r="A284" t="s">
         <v>289</v>
       </c>
-      <c r="B284" s="7">
+      <c r="B284">
         <v>1090</v>
       </c>
-      <c r="C284" s="7">
+      <c r="C284">
         <v>4.3</v>
       </c>
-      <c r="D284" s="7">
+      <c r="D284">
         <v>40.57</v>
       </c>
-      <c r="E284" s="7">
+      <c r="E284">
         <v>84390</v>
       </c>
-      <c r="F284" s="7">
+      <c r="F284">
         <v>1.1000000000000001</v>
       </c>
-      <c r="G284" s="7">
+      <c r="G284">
         <v>23.67</v>
       </c>
-      <c r="H284" s="7">
+      <c r="H284">
         <v>29.39</v>
       </c>
-      <c r="I284" s="7">
+      <c r="I284">
         <v>37.22</v>
       </c>
-      <c r="J284" s="7">
+      <c r="J284">
         <v>48.78</v>
       </c>
-      <c r="K284" s="7">
+      <c r="K284">
         <v>60.31</v>
       </c>
-      <c r="L284" s="7">
+      <c r="L284">
         <v>49240</v>
       </c>
-      <c r="M284" s="7">
+      <c r="M284">
         <v>61120</v>
       </c>
-      <c r="N284" s="7">
+      <c r="N284">
         <v>77420</v>
       </c>
-      <c r="O284" s="7">
+      <c r="O284">
         <v>101460</v>
       </c>
-      <c r="P284" s="7">
+      <c r="P284">
         <v>125450</v>
       </c>
     </row>
@@ -15583,49 +15561,49 @@
       <c r="A285" t="s">
         <v>290</v>
       </c>
-      <c r="B285" s="7">
+      <c r="B285">
         <v>2680</v>
       </c>
-      <c r="C285" s="7">
+      <c r="C285">
         <v>4.5</v>
       </c>
-      <c r="D285" s="7">
+      <c r="D285">
         <v>42.77</v>
       </c>
-      <c r="E285" s="7">
+      <c r="E285">
         <v>88970</v>
       </c>
-      <c r="F285" s="7">
+      <c r="F285">
         <v>4.7</v>
       </c>
-      <c r="G285" s="7">
+      <c r="G285">
         <v>24.42</v>
       </c>
-      <c r="H285" s="7">
+      <c r="H285">
         <v>30.29</v>
       </c>
-      <c r="I285" s="7">
+      <c r="I285">
         <v>37.64</v>
       </c>
-      <c r="J285" s="7">
+      <c r="J285">
         <v>50.27</v>
       </c>
-      <c r="K285" s="7">
+      <c r="K285">
         <v>63.79</v>
       </c>
-      <c r="L285" s="7">
+      <c r="L285">
         <v>50800</v>
       </c>
-      <c r="M285" s="7">
+      <c r="M285">
         <v>63000</v>
       </c>
-      <c r="N285" s="7">
+      <c r="N285">
         <v>78300</v>
       </c>
-      <c r="O285" s="7">
+      <c r="O285">
         <v>104560</v>
       </c>
-      <c r="P285" s="7">
+      <c r="P285">
         <v>132680</v>
       </c>
     </row>

</xml_diff>